<commit_message>
Fix spacing and hide Num anchor link when not needed
</commit_message>
<xml_diff>
--- a/scripts/content-glossary.xlsx
+++ b/scripts/content-glossary.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,6 @@
   <customWorkbookViews>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{CBB582C6-32A4-6D41-A829-2B772B45E7A2}" mergeInterval="0" personalView="1" windowWidth="1821" windowHeight="1108" tabRatio="500" activeSheetId="2"/>
   </customWorkbookViews>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -9611,10 +9610,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T380"/>
+  <dimension ref="A1:T382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A280" sqref="A280:XFD280"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9679,46 +9678,6 @@
       </c>
       <c r="T1" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="80" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="49" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="80" x14ac:dyDescent="0.2">
@@ -22280,6 +22239,46 @@
         <v>41</v>
       </c>
       <c r="H380" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="381" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A381" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B381" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C381" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D381" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F381" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H381" s="49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="382" spans="1:19" ht="80" x14ac:dyDescent="0.2">
+      <c r="A382" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B382" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C382" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D382" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F382" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H382" s="49" t="s">
         <v>36</v>
       </c>
     </row>
@@ -22809,12 +22808,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BA4226224A91A458A707B985AD876EC" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed01e9182d02e6396002211733b860a0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40bf7e35-d9dd-4a50-ad73-4911f6fedc6d" xmlns:ns3="8e019ee6-059a-45f0-b3eb-3e71c24a64f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b7571458447d247cfd0ae7e30923c405" ns2:_="" ns3:_="">
     <xsd:import namespace="40bf7e35-d9dd-4a50-ad73-4911f6fedc6d"/>
@@ -22981,7 +22974,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -22990,24 +22983,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B2A7D17-D1EA-4DBD-A311-F573A50148F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8e019ee6-059a-45f0-b3eb-3e71c24a64f3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="40bf7e35-d9dd-4a50-ad73-4911f6fedc6d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0F0148A-291F-442D-93F2-1BD5EC6516D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23026,10 +23008,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{803E5DCF-739B-486B-8430-6E98EAA83522}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B2A7D17-D1EA-4DBD-A311-F573A50148F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8e019ee6-059a-45f0-b3eb-3e71c24a64f3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="40bf7e35-d9dd-4a50-ad73-4911f6fedc6d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>